<commit_message>
Fixed bug with writing to gitignore (wasn't registering newline character)
</commit_message>
<xml_diff>
--- a/helpers/jargon_example_data.xlsx
+++ b/helpers/jargon_example_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\charlie.sharman\Documents\! Speech to Text\charliesharmanwork\UtterlyVoice_CWS\helpers\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{289E7373-0898-438B-9147-66B69B1A8C71}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D448D65B-A676-4CAE-BF8E-D26530823520}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14295" yWindow="720" windowWidth="14610" windowHeight="14865" xr2:uid="{779ACED3-6C95-4648-8680-90CEC52C5A4F}"/>
+    <workbookView xWindow="-120" yWindow="600" windowWidth="29040" windowHeight="15000" xr2:uid="{779ACED3-6C95-4648-8680-90CEC52C5A4F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>command</t>
   </si>
@@ -54,6 +54,12 @@
   </si>
   <si>
     <t>An example description for a jargon word</t>
+  </si>
+  <si>
+    <t>text</t>
+  </si>
+  <si>
+    <t>this is what the program will write</t>
   </si>
 </sst>
 </file>
@@ -434,20 +440,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8BAB445A-936C-4F47-8DFA-38440EA1B0CA}">
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C15" sqref="C15"/>
+      <selection pane="bottomLeft" activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="2" width="18.28515625" customWidth="1"/>
     <col min="3" max="3" width="39.7109375" customWidth="1"/>
+    <col min="4" max="4" width="33.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -457,8 +464,11 @@
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
+      <c r="D1" s="1" t="s">
+        <v>6</v>
+      </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -467,6 +477,9 @@
       </c>
       <c r="C2" t="s">
         <v>5</v>
+      </c>
+      <c r="D2" t="s">
+        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>